<commit_message>
DRB main file cleaning: removal of partial joints of drug and sample IDs
</commit_message>
<xml_diff>
--- a/data/logs/global_summaries_rows_by_cols.xlsx
+++ b/data/logs/global_summaries_rows_by_cols.xlsx
@@ -8,21 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5147dea5b81ac1f3/04. BNCL (Research Assistant)/Collaborations/Vera Pancaldi collaboration/DNABarcode-DrugFingerprint/data/logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_F91F61DBA6003C162C97AC7154D93B1F79BE6C64" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{852742AA-D9E5-4568-961B-18ED726A11E6}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_F91F61DBA6003C162C97AC7154D93B1F79BE6C64" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0226DC9-4CCD-49A1-B93F-DB6AA3E6784C}"/>
   <bookViews>
-    <workbookView xWindow="9420" yWindow="0" windowWidth="9780" windowHeight="10800" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kept" sheetId="1" r:id="rId1"/>
     <sheet name="discarded" sheetId="2" r:id="rId2"/>
-    <sheet name="old samples" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Experience Name</t>
   </si>
@@ -109,33 +108,6 @@
   </si>
   <si>
     <t>Barcode matrix contains: 813579 unique barcode IDs, and 16 replicates.</t>
-  </si>
-  <si>
-    <t>Barcode matrix contains: 813579 unique barcode IDs, and 20 replicates.</t>
-  </si>
-  <si>
-    <t>Barcode matrix contains: 869714 unique barcode IDs, and 20 replicates.</t>
-  </si>
-  <si>
-    <t>exp130921_1</t>
-  </si>
-  <si>
-    <t>Barcode matrix contains: 413335 unique barcode IDs, and 17 replicates.</t>
-  </si>
-  <si>
-    <t>Barcode matrix contains: 325562 unique barcode IDs, and 40 replicates.</t>
-  </si>
-  <si>
-    <t>exp211221</t>
-  </si>
-  <si>
-    <t>Barcode matrix contains: 251927 unique barcode IDs, and 80 replicates.</t>
-  </si>
-  <si>
-    <t>exp211221cor</t>
-  </si>
-  <si>
-    <t>Barcode matrix contains: 413335 unique barcode IDs, and 48 replicates.</t>
   </si>
 </sst>
 </file>
@@ -207,17 +179,6 @@
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Experience Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Features"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table5" displayName="Table5" ref="A1:B17" totalsRowShown="0">
-  <autoFilter ref="A1:B17" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Experience Name"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Features"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -504,7 +465,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -668,160 +631,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="23.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>